<commit_message>
DE data now (finally) clean
</commit_message>
<xml_diff>
--- a/in/verifications/decomptes_DE.xlsx
+++ b/in/verifications/decomptes_DE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Nombre</t>
   </si>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,9 +453,10 @@
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -472,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -488,8 +489,10 @@
       <c r="E2" s="1">
         <v>34496</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -505,8 +508,10 @@
       <c r="E3" s="1">
         <v>38150</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -522,8 +527,10 @@
       <c r="E4" s="1">
         <v>43861</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -531,33 +538,37 @@
         <v>7</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>40884</v>
+      </c>
+      <c r="E5" s="1">
+        <v>41784</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>79</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>43862</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1">
-        <v>38151</v>
-      </c>
-      <c r="E6" s="1">
-        <v>39970</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -565,33 +576,34 @@
         <v>8</v>
       </c>
       <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>38151</v>
+      </c>
+      <c r="E7" s="1">
+        <v>39970</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>39971</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>43610</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1">
-        <v>38151</v>
-      </c>
-      <c r="E8" s="1">
-        <v>39970</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -599,16 +611,16 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1">
-        <v>39971</v>
+        <v>38151</v>
       </c>
       <c r="E9" s="1">
-        <v>41783</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39970</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -616,33 +628,33 @@
         <v>4</v>
       </c>
       <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>39971</v>
+      </c>
+      <c r="E10" s="1">
+        <v>41783</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
         <v>15</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>41784</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>43610</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1">
-        <v>38151</v>
-      </c>
-      <c r="E11" s="1">
-        <v>39970</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -650,33 +662,33 @@
         <v>9</v>
       </c>
       <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>38151</v>
+      </c>
+      <c r="E12" s="1">
+        <v>39970</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
         <v>5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>39971</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>43610</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1">
-        <v>38151</v>
-      </c>
-      <c r="E13" s="1">
-        <v>39970</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -684,33 +696,33 @@
         <v>10</v>
       </c>
       <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>38151</v>
+      </c>
+      <c r="E14" s="1">
+        <v>39970</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
-      </c>
-      <c r="D14" s="1">
-        <v>39971</v>
-      </c>
-      <c r="E14" s="1">
-        <v>43610</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15" s="1">
-        <v>38151</v>
+        <v>39971</v>
       </c>
       <c r="E15" s="1">
-        <v>39970</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -718,27 +730,27 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1">
-        <v>39971</v>
+        <v>38151</v>
       </c>
       <c r="E16" s="1">
-        <v>43610</v>
+        <v>39970</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1">
-        <v>38151</v>
+        <v>39971</v>
       </c>
       <c r="E17" s="1">
         <v>43610</v>
@@ -746,13 +758,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1">
         <v>38151</v>
@@ -763,18 +775,35 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1">
         <v>38151</v>
       </c>
       <c r="E19" s="1">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>38151</v>
+      </c>
+      <c r="E20" s="1">
         <v>43610</v>
       </c>
     </row>
@@ -788,7 +817,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>